<commit_message>
Removing the if statement to check if a given row is empty, thanks  to that region that is being computed can have empty rows, just like in 3.xlsx
</commit_message>
<xml_diff>
--- a/FileFolder/3.xlsx
+++ b/FileFolder/3.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\worek\gitHub\excelPlayground\FileFolder\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="guardrail" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -178,7 +173,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -355,7 +350,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -364,13 +359,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -502,7 +500,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K8">
-        <v>2323</v>
+        <v>2222222</v>
       </c>
       <c r="L8">
         <v>-60</v>
@@ -536,7 +534,296 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>3123</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11">
+        <v>130</v>
+      </c>
+      <c r="N11">
+        <v>20</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" ref="O11:O18" si="1">M11-L11</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>3123</v>
+      </c>
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="M12">
+        <v>130</v>
+      </c>
+      <c r="N12">
+        <v>20</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>3123</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13">
+        <v>130</v>
+      </c>
+      <c r="N13">
+        <v>20</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>322456</v>
+      </c>
+      <c r="L14">
+        <v>120</v>
+      </c>
+      <c r="M14">
+        <v>110</v>
+      </c>
+      <c r="N14">
+        <v>40</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>3456</v>
+      </c>
+      <c r="L15">
+        <v>120</v>
+      </c>
+      <c r="M15">
+        <v>110</v>
+      </c>
+      <c r="N15">
+        <v>40</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>111</v>
+      </c>
+      <c r="L16">
+        <v>-60</v>
+      </c>
+      <c r="M16">
+        <v>-10</v>
+      </c>
+      <c r="N16">
+        <v>30</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>2323</v>
+      </c>
+      <c r="L17">
+        <v>-60</v>
+      </c>
+      <c r="M17">
+        <v>-10</v>
+      </c>
+      <c r="N17">
+        <v>30</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>3969</v>
+      </c>
+      <c r="L18">
+        <v>-70</v>
+      </c>
+      <c r="M18">
+        <v>-60</v>
+      </c>
+      <c r="N18">
+        <v>30</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>3123</v>
+      </c>
+      <c r="L20">
+        <v>100</v>
+      </c>
+      <c r="M20">
+        <v>130</v>
+      </c>
+      <c r="N20">
+        <v>20</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" ref="O20:O27" si="2">M20-L20</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>3123</v>
+      </c>
+      <c r="L21">
+        <v>100</v>
+      </c>
+      <c r="M21">
+        <v>130</v>
+      </c>
+      <c r="N21">
+        <v>20</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>1111</v>
+      </c>
+      <c r="L22">
+        <v>100</v>
+      </c>
+      <c r="M22">
+        <v>130</v>
+      </c>
+      <c r="N22">
+        <v>20</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>3456</v>
+      </c>
+      <c r="L23">
+        <v>120</v>
+      </c>
+      <c r="M23">
+        <v>110</v>
+      </c>
+      <c r="N23">
+        <v>40</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="24" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>3456</v>
+      </c>
+      <c r="L24">
+        <v>120</v>
+      </c>
+      <c r="M24">
+        <v>110</v>
+      </c>
+      <c r="N24">
+        <v>40</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="25" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>444444444</v>
+      </c>
+      <c r="L25">
+        <v>-60</v>
+      </c>
+      <c r="M25">
+        <v>-10</v>
+      </c>
+      <c r="N25">
+        <v>30</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>33333333333</v>
+      </c>
+      <c r="L26">
+        <v>-60</v>
+      </c>
+      <c r="M26">
+        <v>-10</v>
+      </c>
+      <c r="N26">
+        <v>30</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>3969</v>
+      </c>
+      <c r="L27">
+        <v>-70</v>
+      </c>
+      <c r="M27">
+        <v>-60</v>
+      </c>
+      <c r="N27">
+        <v>30</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>